<commit_message>
refactored for data gathering
</commit_message>
<xml_diff>
--- a/Community/data.xlsx
+++ b/Community/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="28">
   <si>
     <t>Karate</t>
   </si>
@@ -67,6 +67,48 @@
   </si>
   <si>
     <t>Football</t>
+  </si>
+  <si>
+    <t>fitness</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>REGULAR/S-</t>
+  </si>
+  <si>
+    <t>CLIQUE/S-</t>
+  </si>
+  <si>
+    <t>REGULAR/S+</t>
+  </si>
+  <si>
+    <t>CLIQUE/S+</t>
+  </si>
+  <si>
+    <t>times R-</t>
+  </si>
+  <si>
+    <t>times Q-</t>
+  </si>
+  <si>
+    <t>times R+</t>
+  </si>
+  <si>
+    <t>times Q+</t>
+  </si>
+  <si>
+    <t>fit R-</t>
+  </si>
+  <si>
+    <t>fit Q-</t>
+  </si>
+  <si>
+    <t>fit R+</t>
+  </si>
+  <si>
+    <t>fit Q+</t>
   </si>
 </sst>
 </file>
@@ -511,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A65" sqref="A65:C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -663,7 +705,7 @@
         <v>115</v>
       </c>
       <c r="C10" s="5">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5">
@@ -701,7 +743,7 @@
       </c>
       <c r="C12" s="5">
         <f>C10 - AVERAGE(F10:F14)</f>
-        <v>120.60000000000002</v>
+        <v>123.60000000000002</v>
       </c>
       <c r="D12" s="5">
         <f>AVERAGE(G10:G14)</f>
@@ -725,7 +767,7 @@
       </c>
       <c r="C13" s="7">
         <f xml:space="preserve"> (C10-C12)/C10</f>
-        <v>0.80326264274061987</v>
+        <v>0.79935064935064937</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="11">
@@ -1555,12 +1597,749 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5">
+        <v>34</v>
+      </c>
+      <c r="C2" s="5">
+        <v>78</v>
+      </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="5">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="G2" s="11">
+        <v>0.40699999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="5">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.41199999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="5">
+        <v>115</v>
+      </c>
+      <c r="C9" s="5">
+        <v>616</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="5">
+        <v>3.4161000000000001</v>
+      </c>
+      <c r="G9" s="11">
+        <v>0.55449999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.15379999999999999</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.56630000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" t="s">
+        <v>23</v>
+      </c>
+      <c r="N15" t="s">
+        <v>24</v>
+      </c>
+      <c r="O15" t="s">
+        <v>25</v>
+      </c>
+      <c r="P15" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="5">
+        <v>4039</v>
+      </c>
+      <c r="C16" s="5">
+        <v>88234</v>
+      </c>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="5">
+        <v>903.00840000000005</v>
+      </c>
+      <c r="G16" s="11">
+        <v>0.55369999999999997</v>
+      </c>
+      <c r="I16">
+        <v>884.69989999999996</v>
+      </c>
+      <c r="J16">
+        <v>178.1489</v>
+      </c>
+      <c r="N16">
+        <v>0.53149999999999997</v>
+      </c>
+      <c r="O16">
+        <v>0.77510000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="5">
+        <v>179.95490000000001</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0.77080000000000004</v>
+      </c>
+      <c r="I17">
+        <v>1039.4963</v>
+      </c>
+      <c r="J17">
+        <v>159.0831</v>
+      </c>
+      <c r="N17">
+        <v>0.54520000000000002</v>
+      </c>
+      <c r="O17">
+        <v>0.76959999999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="I18">
+        <v>979.60299999999995</v>
+      </c>
+      <c r="J18">
+        <v>242.6739</v>
+      </c>
+      <c r="N18">
+        <v>0.55189999999999995</v>
+      </c>
+      <c r="O18">
+        <v>0.77839999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="I19">
+        <v>852.4144</v>
+      </c>
+      <c r="J19">
+        <v>157.43100000000001</v>
+      </c>
+      <c r="N19">
+        <v>0.5847</v>
+      </c>
+      <c r="O19">
+        <v>0.76729999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>758.82809999999995</v>
+      </c>
+      <c r="J20">
+        <v>162.4374</v>
+      </c>
+      <c r="N20">
+        <v>0.55520000000000003</v>
+      </c>
+      <c r="O20">
+        <v>0.76359999999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" s="5">
+        <v>22963</v>
+      </c>
+      <c r="C23" s="5">
+        <v>48436</v>
+      </c>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="5"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="5">
+        <v>4941</v>
+      </c>
+      <c r="C30" s="5">
+        <v>6594</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="5"/>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="5"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="5">
+        <v>334863</v>
+      </c>
+      <c r="C37" s="5">
+        <v>925872</v>
+      </c>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="5"/>
+      <c r="G37" s="11"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="5">
+        <v>1134890</v>
+      </c>
+      <c r="C44" s="5">
+        <v>2987624</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="5"/>
+      <c r="G44" s="11"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="5"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B51" s="5">
+        <v>36692</v>
+      </c>
+      <c r="C51" s="5">
+        <v>183831</v>
+      </c>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F51" s="5"/>
+      <c r="G51" s="11"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5"/>
+    </row>
+    <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G57" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="5">
+        <v>18772</v>
+      </c>
+      <c r="C58" s="5">
+        <v>198110</v>
+      </c>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F58" s="5"/>
+      <c r="G58" s="11"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more text and data
</commit_message>
<xml_diff>
--- a/Community/data.xlsx
+++ b/Community/data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="50">
   <si>
     <t>Karate</t>
   </si>
@@ -133,6 +133,48 @@
   </si>
   <si>
     <t>coms Q+</t>
+  </si>
+  <si>
+    <t>com Q-</t>
+  </si>
+  <si>
+    <t>REGULAR/S- 9</t>
+  </si>
+  <si>
+    <t>CLIQUE/S- 9</t>
+  </si>
+  <si>
+    <t>times R- 9</t>
+  </si>
+  <si>
+    <t>times Q- 9</t>
+  </si>
+  <si>
+    <t>fit R- 9</t>
+  </si>
+  <si>
+    <t>fit Q- 9</t>
+  </si>
+  <si>
+    <t>gens R- 9</t>
+  </si>
+  <si>
+    <t>gens Q- 9</t>
+  </si>
+  <si>
+    <t>coms R- 9</t>
+  </si>
+  <si>
+    <t>coms Q- 9</t>
+  </si>
+  <si>
+    <t>CLIQUE/S- 4</t>
+  </si>
+  <si>
+    <t>no conv</t>
+  </si>
+  <si>
+    <t>10min</t>
   </si>
 </sst>
 </file>
@@ -577,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1621,10 +1663,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA61"/>
+  <dimension ref="A1:AA62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Z21" sqref="Z21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="U56" sqref="U56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2479,6 +2521,9 @@
       <c r="J16">
         <v>28.502700000000001</v>
       </c>
+      <c r="K16">
+        <v>714.78210000000001</v>
+      </c>
       <c r="L16">
         <v>400.18979999999999</v>
       </c>
@@ -2488,6 +2533,9 @@
       <c r="O16">
         <v>0.81330000000000002</v>
       </c>
+      <c r="P16">
+        <v>0.72660000000000002</v>
+      </c>
       <c r="Q16">
         <v>0.82220000000000004</v>
       </c>
@@ -2497,6 +2545,9 @@
       <c r="T16">
         <v>68</v>
       </c>
+      <c r="U16">
+        <v>2</v>
+      </c>
       <c r="V16">
         <v>7</v>
       </c>
@@ -2505,6 +2556,9 @@
       </c>
       <c r="Y16">
         <v>32</v>
+      </c>
+      <c r="Z16">
+        <v>76</v>
       </c>
       <c r="AA16">
         <v>19</v>
@@ -2530,6 +2584,9 @@
       <c r="J17">
         <v>18.969899999999999</v>
       </c>
+      <c r="K17">
+        <v>710.55439999999999</v>
+      </c>
       <c r="L17">
         <v>399.07900000000001</v>
       </c>
@@ -2539,6 +2596,9 @@
       <c r="O17">
         <v>0.78520000000000001</v>
       </c>
+      <c r="P17">
+        <v>0.71889999999999998</v>
+      </c>
       <c r="Q17">
         <v>0.81830000000000003</v>
       </c>
@@ -2548,6 +2608,9 @@
       <c r="T17">
         <v>49</v>
       </c>
+      <c r="U17">
+        <v>3</v>
+      </c>
       <c r="V17">
         <v>7</v>
       </c>
@@ -2556,6 +2619,9 @@
       </c>
       <c r="Y17">
         <v>37</v>
+      </c>
+      <c r="Z17">
+        <v>58</v>
       </c>
       <c r="AA17">
         <v>23</v>
@@ -2569,14 +2635,21 @@
       <c r="E18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
+      <c r="F18" s="5">
+        <v>699.44259999999997</v>
+      </c>
+      <c r="G18" s="5">
+        <v>0.7339</v>
+      </c>
       <c r="I18">
         <v>302.1891</v>
       </c>
       <c r="J18">
         <v>13.634600000000001</v>
       </c>
+      <c r="K18">
+        <v>715.33280000000002</v>
+      </c>
       <c r="L18">
         <v>357.43779999999998</v>
       </c>
@@ -2586,6 +2659,9 @@
       <c r="O18">
         <v>0.79610000000000003</v>
       </c>
+      <c r="P18">
+        <v>0.73509999999999998</v>
+      </c>
       <c r="Q18">
         <v>0.81969999999999998</v>
       </c>
@@ -2595,6 +2671,9 @@
       <c r="T18">
         <v>34</v>
       </c>
+      <c r="U18">
+        <v>3</v>
+      </c>
       <c r="V18">
         <v>6</v>
       </c>
@@ -2603,6 +2682,9 @@
       </c>
       <c r="Y18">
         <v>29</v>
+      </c>
+      <c r="Z18">
+        <v>88</v>
       </c>
       <c r="AA18">
         <v>17</v>
@@ -2628,6 +2710,9 @@
       <c r="J19">
         <v>23.719200000000001</v>
       </c>
+      <c r="K19">
+        <v>702.25930000000005</v>
+      </c>
       <c r="L19">
         <v>404.1164</v>
       </c>
@@ -2637,6 +2722,9 @@
       <c r="O19">
         <v>0.80700000000000005</v>
       </c>
+      <c r="P19">
+        <v>0.75390000000000001</v>
+      </c>
       <c r="Q19">
         <v>0.82399999999999995</v>
       </c>
@@ -2646,6 +2734,9 @@
       <c r="T19">
         <v>59</v>
       </c>
+      <c r="U19">
+        <v>3</v>
+      </c>
       <c r="V19">
         <v>7</v>
       </c>
@@ -2654,6 +2745,9 @@
       </c>
       <c r="Y19">
         <v>32</v>
+      </c>
+      <c r="Z19">
+        <v>72</v>
       </c>
       <c r="AA19">
         <v>16</v>
@@ -2666,6 +2760,9 @@
       <c r="J20">
         <v>34.441499999999998</v>
       </c>
+      <c r="K20">
+        <v>654.28409999999997</v>
+      </c>
       <c r="L20">
         <v>398.45670000000001</v>
       </c>
@@ -2675,6 +2772,9 @@
       <c r="O20">
         <v>0.80369999999999997</v>
       </c>
+      <c r="P20">
+        <v>0.73509999999999998</v>
+      </c>
       <c r="Q20">
         <v>0.82579999999999998</v>
       </c>
@@ -2684,6 +2784,9 @@
       <c r="T20">
         <v>89</v>
       </c>
+      <c r="U20">
+        <v>3</v>
+      </c>
       <c r="V20">
         <v>7</v>
       </c>
@@ -2692,6 +2795,9 @@
       </c>
       <c r="Y20">
         <v>29</v>
+      </c>
+      <c r="Z20">
+        <v>78</v>
       </c>
       <c r="AA20">
         <v>18</v>
@@ -2714,6 +2820,54 @@
       <c r="G22" s="11" t="s">
         <v>14</v>
       </c>
+      <c r="I22" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" t="s">
+        <v>39</v>
+      </c>
+      <c r="L22" t="s">
+        <v>40</v>
+      </c>
+      <c r="N22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O22" t="s">
+        <v>25</v>
+      </c>
+      <c r="P22" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>42</v>
+      </c>
+      <c r="S22" t="s">
+        <v>28</v>
+      </c>
+      <c r="T22" t="s">
+        <v>29</v>
+      </c>
+      <c r="U22" t="s">
+        <v>43</v>
+      </c>
+      <c r="V22" t="s">
+        <v>44</v>
+      </c>
+      <c r="X22" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
@@ -2729,8 +2883,60 @@
       <c r="E23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="11"/>
+      <c r="F23" s="5">
+        <v>331.09</v>
+      </c>
+      <c r="G23" s="11">
+        <v>0.49109999999999998</v>
+      </c>
+      <c r="I23">
+        <v>337.89</v>
+      </c>
+      <c r="J23">
+        <v>334.89510000000001</v>
+      </c>
+      <c r="K23">
+        <v>132.26820000000001</v>
+      </c>
+      <c r="L23">
+        <v>135.65110000000001</v>
+      </c>
+      <c r="N23">
+        <v>0.48530000000000001</v>
+      </c>
+      <c r="O23">
+        <v>0.50980000000000003</v>
+      </c>
+      <c r="P23">
+        <v>0.4743</v>
+      </c>
+      <c r="Q23">
+        <v>0.49049999999999999</v>
+      </c>
+      <c r="S23">
+        <v>15</v>
+      </c>
+      <c r="T23">
+        <v>15</v>
+      </c>
+      <c r="U23">
+        <v>15</v>
+      </c>
+      <c r="V23">
+        <v>14</v>
+      </c>
+      <c r="X23">
+        <v>1004</v>
+      </c>
+      <c r="Y23">
+        <v>865</v>
+      </c>
+      <c r="Z23">
+        <v>1014</v>
+      </c>
+      <c r="AA23">
+        <v>871</v>
+      </c>
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
@@ -2740,8 +2946,60 @@
       <c r="E24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
+      <c r="F24" s="5">
+        <v>344.8365</v>
+      </c>
+      <c r="G24" s="5">
+        <v>0.50839999999999996</v>
+      </c>
+      <c r="I24">
+        <v>349.23919999999998</v>
+      </c>
+      <c r="J24">
+        <v>354.7944</v>
+      </c>
+      <c r="K24">
+        <v>143.3236</v>
+      </c>
+      <c r="L24">
+        <v>130.46719999999999</v>
+      </c>
+      <c r="N24">
+        <v>0.49709999999999999</v>
+      </c>
+      <c r="O24">
+        <v>0.50739999999999996</v>
+      </c>
+      <c r="P24">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="Q24">
+        <v>0.49359999999999998</v>
+      </c>
+      <c r="S24">
+        <v>15</v>
+      </c>
+      <c r="T24">
+        <v>15</v>
+      </c>
+      <c r="U24">
+        <v>15</v>
+      </c>
+      <c r="V24">
+        <v>15</v>
+      </c>
+      <c r="X24">
+        <v>968</v>
+      </c>
+      <c r="Y24">
+        <v>887</v>
+      </c>
+      <c r="Z24">
+        <v>972</v>
+      </c>
+      <c r="AA24">
+        <v>898</v>
+      </c>
     </row>
     <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
@@ -2749,10 +3007,62 @@
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="F25" s="5">
+        <v>135.33250000000001</v>
+      </c>
+      <c r="G25" s="5">
+        <v>0.47510000000000002</v>
+      </c>
+      <c r="I25">
+        <v>333.39780000000002</v>
+      </c>
+      <c r="J25">
+        <v>348.24209999999999</v>
+      </c>
+      <c r="K25">
+        <v>147.33000000000001</v>
+      </c>
+      <c r="L25">
+        <v>133.0941</v>
+      </c>
+      <c r="N25">
+        <v>0.49540000000000001</v>
+      </c>
+      <c r="O25">
+        <v>0.5091</v>
+      </c>
+      <c r="P25">
+        <v>0.47689999999999999</v>
+      </c>
+      <c r="Q25">
+        <v>0.49070000000000003</v>
+      </c>
+      <c r="S25">
+        <v>16</v>
+      </c>
+      <c r="T25">
+        <v>15</v>
+      </c>
+      <c r="U25">
+        <v>15</v>
+      </c>
+      <c r="V25">
+        <v>15</v>
+      </c>
+      <c r="X25">
+        <v>950</v>
+      </c>
+      <c r="Y25">
+        <v>891</v>
+      </c>
+      <c r="Z25">
+        <v>1023</v>
+      </c>
+      <c r="AA25">
+        <v>907</v>
+      </c>
     </row>
     <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
@@ -2760,10 +3070,112 @@
       <c r="C26" s="7"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="F26" s="5">
+        <v>138.23269999999999</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0.49109999999999998</v>
+      </c>
+      <c r="I26">
+        <v>287.24590000000001</v>
+      </c>
+      <c r="J26">
+        <v>341.26990000000001</v>
+      </c>
+      <c r="K26">
+        <v>134.1985</v>
+      </c>
+      <c r="L26">
+        <v>156.58070000000001</v>
+      </c>
+      <c r="N26">
+        <v>0.4819</v>
+      </c>
+      <c r="O26">
+        <v>0.51060000000000005</v>
+      </c>
+      <c r="P26">
+        <v>0.4743</v>
+      </c>
+      <c r="Q26">
+        <v>0.49159999999999998</v>
+      </c>
+      <c r="S26">
+        <v>15</v>
+      </c>
+      <c r="T26">
+        <v>15</v>
+      </c>
+      <c r="U26">
+        <v>12</v>
+      </c>
+      <c r="V26">
+        <v>15</v>
+      </c>
+      <c r="X26">
+        <v>1020</v>
+      </c>
+      <c r="Y26">
+        <v>924</v>
+      </c>
+      <c r="Z26">
+        <v>967</v>
+      </c>
+      <c r="AA26">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>348.67720000000003</v>
+      </c>
+      <c r="J27">
+        <v>344.98110000000003</v>
+      </c>
+      <c r="K27">
+        <v>119.5423</v>
+      </c>
+      <c r="L27">
+        <v>135.37020000000001</v>
+      </c>
+      <c r="N27">
+        <v>0.49590000000000001</v>
+      </c>
+      <c r="O27">
+        <v>0.50529999999999997</v>
+      </c>
+      <c r="P27">
+        <v>0.47489999999999999</v>
+      </c>
+      <c r="Q27">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="S27">
+        <v>17</v>
+      </c>
+      <c r="T27">
+        <v>15</v>
+      </c>
+      <c r="U27">
+        <v>15</v>
+      </c>
+      <c r="V27">
+        <v>15</v>
+      </c>
+      <c r="X27">
+        <v>973</v>
+      </c>
+      <c r="Y27">
+        <v>862</v>
+      </c>
+      <c r="Z27">
+        <v>1007</v>
+      </c>
+      <c r="AA27">
+        <v>923</v>
+      </c>
     </row>
     <row r="28" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:27" x14ac:dyDescent="0.25">
@@ -2788,47 +3200,23 @@
       <c r="J29" t="s">
         <v>21</v>
       </c>
-      <c r="K29" t="s">
-        <v>22</v>
-      </c>
-      <c r="L29" t="s">
-        <v>23</v>
-      </c>
       <c r="N29" t="s">
         <v>24</v>
       </c>
       <c r="O29" t="s">
         <v>25</v>
       </c>
-      <c r="P29" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>27</v>
-      </c>
       <c r="S29" t="s">
         <v>28</v>
       </c>
       <c r="T29" t="s">
         <v>29</v>
       </c>
-      <c r="U29" t="s">
-        <v>30</v>
-      </c>
-      <c r="V29" t="s">
-        <v>31</v>
-      </c>
       <c r="X29" t="s">
         <v>32</v>
       </c>
       <c r="Y29" t="s">
         <v>33</v>
-      </c>
-      <c r="Z29" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA29" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.25">
@@ -2845,8 +3233,36 @@
       <c r="E30" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="5"/>
-      <c r="G30" s="11"/>
+      <c r="F30" s="5">
+        <v>264.60019999999997</v>
+      </c>
+      <c r="G30" s="11">
+        <v>0.78220000000000001</v>
+      </c>
+      <c r="I30">
+        <v>255.4708</v>
+      </c>
+      <c r="J30">
+        <v>84.111800000000002</v>
+      </c>
+      <c r="N30">
+        <v>0.77959999999999996</v>
+      </c>
+      <c r="O30">
+        <v>0.76380000000000003</v>
+      </c>
+      <c r="S30">
+        <v>307</v>
+      </c>
+      <c r="T30">
+        <v>123</v>
+      </c>
+      <c r="X30">
+        <v>567</v>
+      </c>
+      <c r="Y30">
+        <v>664</v>
+      </c>
     </row>
     <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
@@ -2856,33 +3272,131 @@
       <c r="E31" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
+      <c r="F31" s="5">
+        <v>144.9263</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0.7893</v>
+      </c>
+      <c r="I31">
+        <v>277.94130000000001</v>
+      </c>
+      <c r="J31">
+        <v>117.95350000000001</v>
+      </c>
+      <c r="N31">
+        <v>0.7823</v>
+      </c>
+      <c r="O31">
+        <v>0.78510000000000002</v>
+      </c>
+      <c r="S31">
+        <v>334</v>
+      </c>
+      <c r="T31">
+        <v>168</v>
+      </c>
+      <c r="X31">
+        <v>563</v>
+      </c>
+      <c r="Y31">
+        <v>593</v>
+      </c>
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>301.48970000000003</v>
+      </c>
+      <c r="J32">
+        <v>167.6849</v>
+      </c>
+      <c r="N32">
+        <v>0.79049999999999998</v>
+      </c>
+      <c r="O32">
+        <v>0.79930000000000001</v>
+      </c>
+      <c r="S32">
+        <v>365</v>
+      </c>
+      <c r="T32">
+        <v>232</v>
+      </c>
+      <c r="X32">
+        <v>544</v>
+      </c>
+      <c r="Y32">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>230.5264</v>
+      </c>
+      <c r="J33">
+        <v>148.9872</v>
+      </c>
+      <c r="N33">
+        <v>0.77349999999999997</v>
+      </c>
+      <c r="O33">
+        <v>0.78680000000000005</v>
+      </c>
+      <c r="S33">
+        <v>281</v>
+      </c>
+      <c r="T33">
+        <v>213</v>
+      </c>
+      <c r="X33">
+        <v>586</v>
+      </c>
+      <c r="Y33">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>257.5729</v>
+      </c>
+      <c r="J34">
+        <v>205.8939</v>
+      </c>
+      <c r="N34">
+        <v>0.78490000000000004</v>
+      </c>
+      <c r="O34">
+        <v>0.81169999999999998</v>
+      </c>
+      <c r="S34">
+        <v>312</v>
+      </c>
+      <c r="T34">
+        <v>286</v>
+      </c>
+      <c r="X34">
+        <v>551</v>
+      </c>
+      <c r="Y34">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="2" t="s">
         <v>1</v>
@@ -2898,8 +3412,20 @@
       <c r="G36" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>21</v>
+      </c>
+      <c r="J36" t="s">
+        <v>25</v>
+      </c>
+      <c r="K36" t="s">
+        <v>29</v>
+      </c>
+      <c r="L36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>9</v>
       </c>
@@ -2910,47 +3436,41 @@
         <v>925872</v>
       </c>
       <c r="D37" s="5"/>
-      <c r="E37" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="11"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
       <c r="E38" s="5" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
-      <c r="E39" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="5"/>
-      <c r="E40" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
     </row>
-    <row r="42" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="2" t="s">
         <v>1</v>
@@ -2966,8 +3486,20 @@
       <c r="G43" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I43" t="s">
+        <v>21</v>
+      </c>
+      <c r="J43" t="s">
+        <v>25</v>
+      </c>
+      <c r="K43" t="s">
+        <v>29</v>
+      </c>
+      <c r="L43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>10</v>
       </c>
@@ -2978,47 +3510,40 @@
         <v>2987624</v>
       </c>
       <c r="D44" s="5"/>
-      <c r="E44" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="F44" s="5"/>
       <c r="G44" s="11"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="5" t="s">
-        <v>17</v>
+        <v>47</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
-      <c r="E46" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="5"/>
-      <c r="E47" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="E47" s="5"/>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
     </row>
-    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="2" t="s">
         <v>1</v>
@@ -3034,8 +3559,32 @@
       <c r="G50" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I50" t="s">
+        <v>20</v>
+      </c>
+      <c r="J50" t="s">
+        <v>21</v>
+      </c>
+      <c r="N50" t="s">
+        <v>24</v>
+      </c>
+      <c r="O50" t="s">
+        <v>25</v>
+      </c>
+      <c r="S50" t="s">
+        <v>28</v>
+      </c>
+      <c r="T50" t="s">
+        <v>29</v>
+      </c>
+      <c r="X50" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>11</v>
       </c>
@@ -3047,46 +3596,112 @@
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="5" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="F51" s="5"/>
       <c r="G51" s="11"/>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J51">
+        <v>621.18010000000004</v>
+      </c>
+      <c r="O51">
+        <v>0.37309999999999999</v>
+      </c>
+      <c r="T51">
+        <v>54</v>
+      </c>
+      <c r="Y51">
+        <v>1727</v>
+      </c>
+    </row>
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
-      <c r="B52" s="5"/>
+      <c r="B52" s="5" t="s">
+        <v>48</v>
+      </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F52" s="5">
+        <v>616.07730000000004</v>
+      </c>
+      <c r="G52" s="5">
+        <v>0.3614</v>
+      </c>
+      <c r="J52">
+        <v>613.9502</v>
+      </c>
+      <c r="O52">
+        <v>0.35980000000000001</v>
+      </c>
+      <c r="T52">
+        <v>49</v>
+      </c>
+      <c r="Y52">
+        <v>1794</v>
+      </c>
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
+      <c r="B53" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
-      <c r="E53" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="E53" s="5"/>
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J53">
+        <v>614.13840000000005</v>
+      </c>
+      <c r="O53">
+        <v>0.35659999999999997</v>
+      </c>
+      <c r="T53">
+        <v>48</v>
+      </c>
+      <c r="Y53">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="E54" s="5"/>
       <c r="F54" s="5"/>
       <c r="G54" s="5"/>
-    </row>
-    <row r="56" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J54">
+        <v>614.577</v>
+      </c>
+      <c r="O54">
+        <v>0.35680000000000001</v>
+      </c>
+      <c r="T54">
+        <v>51</v>
+      </c>
+      <c r="Y54">
+        <v>1769</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="J55">
+        <v>616.54070000000002</v>
+      </c>
+      <c r="O55">
+        <v>0.36070000000000002</v>
+      </c>
+      <c r="T55">
+        <v>57</v>
+      </c>
+      <c r="Y55">
+        <v>1801</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="2" t="s">
         <v>1</v>
@@ -3102,8 +3717,20 @@
       <c r="G57" s="11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I57" t="s">
+        <v>21</v>
+      </c>
+      <c r="J57" t="s">
+        <v>25</v>
+      </c>
+      <c r="K57" t="s">
+        <v>29</v>
+      </c>
+      <c r="L57" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>12</v>
       </c>
@@ -3114,13 +3741,23 @@
         <v>198110</v>
       </c>
       <c r="D58" s="5"/>
-      <c r="E58" s="5" t="s">
-        <v>16</v>
-      </c>
+      <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="11"/>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I58">
+        <v>123.6211</v>
+      </c>
+      <c r="J58">
+        <v>0.46660000000000001</v>
+      </c>
+      <c r="K58">
+        <v>31</v>
+      </c>
+      <c r="L58">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="5"/>
       <c r="C59" s="5"/>
@@ -3128,30 +3765,80 @@
       <c r="E59" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F59" s="5">
+        <v>134.90989999999999</v>
+      </c>
+      <c r="G59" s="5">
+        <v>0.46029999999999999</v>
+      </c>
+      <c r="I59">
+        <v>129.93809999999999</v>
+      </c>
+      <c r="J59">
+        <v>0.45960000000000001</v>
+      </c>
+      <c r="K59">
+        <v>33</v>
+      </c>
+      <c r="L59">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A60" s="5"/>
       <c r="B60" s="5"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
-      <c r="E60" s="5" t="s">
-        <v>18</v>
-      </c>
+      <c r="E60" s="5"/>
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I60">
+        <v>75.951700000000002</v>
+      </c>
+      <c r="J60">
+        <v>0.44679999999999997</v>
+      </c>
+      <c r="K60">
+        <v>20</v>
+      </c>
+      <c r="L60">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="5"/>
-      <c r="E61" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="E61" s="5"/>
       <c r="F61" s="5"/>
       <c r="G61" s="5"/>
+      <c r="I61">
+        <v>150.12029999999999</v>
+      </c>
+      <c r="J61">
+        <v>0.47120000000000001</v>
+      </c>
+      <c r="K61">
+        <v>38</v>
+      </c>
+      <c r="L61">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="I62">
+        <v>194.91849999999999</v>
+      </c>
+      <c r="J62">
+        <v>0.45729999999999998</v>
+      </c>
+      <c r="K62">
+        <v>48</v>
+      </c>
+      <c r="L62">
+        <v>604</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>